<commit_message>
add giao dien xem sp trong gio hang
</commit_message>
<xml_diff>
--- a/danh_sach_chuc_nang.xlsx
+++ b/danh_sach_chuc_nang.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ssaan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TTVnienluan\Thuc_tap_viet_nien_luan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FA14D3-1543-467B-93DC-1E359105CBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4346413E-153C-46CD-9215-80F2B58D2C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="35">
   <si>
     <t>Trần Đại Đức</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t>Hồ sơ cá nhân</t>
-  </si>
-  <si>
-    <t>Đức</t>
   </si>
   <si>
     <t>Đổi mật khẩu</t>
@@ -485,7 +482,9 @@
   </sheetPr>
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -504,7 +503,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
@@ -830,16 +829,14 @@
       <c r="F14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="L14" s="5"/>
     </row>
     <row r="15" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>6</v>
@@ -853,16 +850,14 @@
       <c r="F15" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>14</v>
-      </c>
+      <c r="L15" s="2"/>
     </row>
     <row r="16" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>8</v>
@@ -874,18 +869,16 @@
         <v>45</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>15</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="L16" s="2"/>
     </row>
     <row r="17" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>6</v>
@@ -899,16 +892,14 @@
       <c r="F17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="L17" s="2" t="s">
-        <v>24</v>
-      </c>
+      <c r="L17" s="2"/>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>6</v>
@@ -922,16 +913,14 @@
       <c r="F18" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L18" s="2" t="s">
-        <v>27</v>
-      </c>
+      <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>6</v>
@@ -945,16 +934,14 @@
       <c r="F19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L19" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="L19" s="3"/>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>7</v>
@@ -974,7 +961,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>7</v>

</xml_diff>